<commit_message>
Interrupt timeout, display update, thershold update
</commit_message>
<xml_diff>
--- a/Display.xlsx
+++ b/Display.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ESP Playground\AirQuality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6E72D9-68F3-460E-8060-8FD212E6EDC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752189A7-A1F3-4546-859C-CA1A58AA88E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="2512" windowWidth="21600" windowHeight="11423" activeTab="1" xr2:uid="{640D9A9B-E986-4773-BCDE-A1F2849D844A}"/>
+    <workbookView xWindow="3218" yWindow="3218" windowWidth="21600" windowHeight="11422" activeTab="2" xr2:uid="{640D9A9B-E986-4773-BCDE-A1F2849D844A}"/>
   </bookViews>
   <sheets>
     <sheet name="Engineering Setup" sheetId="1" r:id="rId1"/>
-    <sheet name="User Setup" sheetId="2" r:id="rId2"/>
+    <sheet name="Two Page Setup" sheetId="2" r:id="rId2"/>
+    <sheet name="Single Page Setup" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="107">
   <si>
     <t>BME680</t>
   </si>
@@ -310,6 +311,51 @@
   </si>
   <si>
     <t>Average Pressure Filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Particulate Matter</t>
+  </si>
+  <si>
+    <t>absolute Humidity</t>
+  </si>
+  <si>
+    <t>deltaPressure</t>
+  </si>
+  <si>
+    <t>totalVolotileOrganicCompounds</t>
   </si>
 </sst>
 </file>
@@ -547,7 +593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -580,6 +626,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1766,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5CB0FF-4212-4CC9-93BA-54A050B1D9CE}">
   <dimension ref="A2:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2576,13 +2625,525 @@
         <f>-C35+SQRT(C35*C35+2*C35)</f>
         <v>4.3529912306300694E-3</v>
       </c>
-      <c r="E36">
-        <f>-E35+SQRT(E35*E35+2*E35)</f>
-        <v>3.6347558950161661E-4</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F251BC20-0382-41B6-B660-C0840633F309}">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="26.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="2.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.9296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="19" width="1.73046875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="2.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>0</v>
+      </c>
+      <c r="M1">
+        <v>1</v>
+      </c>
+      <c r="N1">
+        <v>2</v>
+      </c>
+      <c r="O1">
+        <v>3</v>
+      </c>
+      <c r="P1">
+        <v>4</v>
+      </c>
+      <c r="Q1">
+        <v>5</v>
+      </c>
+      <c r="R1">
+        <v>6</v>
+      </c>
+      <c r="S1">
+        <v>7</v>
+      </c>
+      <c r="T1">
+        <v>8</v>
+      </c>
+      <c r="U1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="32"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="3">
+        <v>3</v>
+      </c>
+      <c r="R2" s="3">
+        <v>8</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="3">
+        <v>3</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>2</v>
+      </c>
+      <c r="R3" s="3">
+        <v>5</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" s="3">
+        <v>3</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="N4" s="31"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>5</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S4" s="3">
+        <v>1</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="N5" s="31"/>
+      <c r="O5" s="3">
+        <v>1</v>
+      </c>
+      <c r="P5" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>3</v>
+      </c>
+      <c r="R5" s="3">
+        <v>4</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B7" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B8" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B9" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="34"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B10" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B11" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B12" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B13" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B14" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="34">
+        <v>2</v>
+      </c>
+      <c r="E18" s="34"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>